<commit_message>
Let's handle non-nullable as well
</commit_message>
<xml_diff>
--- a/ExcelORM/ExcelORMTests/testFiles/additionalTypes.xlsx
+++ b/ExcelORM/ExcelORMTests/testFiles/additionalTypes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/piotr/git/ExcelORM/ExcelORM/ExcelORMTests/testFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F87F5506-DDC1-E043-BC5E-B7F60719204F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF0B4AD2-B63A-1E45-8500-3D721B32D341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="660" windowWidth="25440" windowHeight="14500" xr2:uid="{1119CF16-2DAD-E540-B026-39473101B51C}"/>
+    <workbookView xWindow="80" yWindow="660" windowWidth="25440" windowHeight="14460" xr2:uid="{1119CF16-2DAD-E540-B026-39473101B51C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>MyEnum</t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>Second</t>
-  </si>
-  <si>
-    <t>Non existent</t>
   </si>
   <si>
     <t>a3834ef3-96f2-4268-915e-101098b87151</t>
@@ -434,7 +431,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -452,7 +449,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -460,15 +457,15 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>